<commit_message>
Added SelectHotelPage and room count validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eccd6de18900521a/Desktop/FLM testing/POM/FrameworkPOM-master/src/test/resources/testdata/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{2CC5B2EA-2537-4007-ABD4-67673B59F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{435FD138-A5BD-4544-B14D-22F3DC38A764}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{2CC5B2EA-2537-4007-ABD4-67673B59F46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C64B2454-8B07-426E-9C48-6AF88FD38C64}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01F410BB-4CDF-4E65-BF55-31489716C62E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="43">
   <si>
     <t>TC101</t>
   </si>
@@ -157,6 +157,15 @@
   </si>
   <si>
     <t>15/02/2026</t>
+  </si>
+  <si>
+    <t>27/02/2026</t>
+  </si>
+  <si>
+    <t>TC06</t>
+  </si>
+  <si>
+    <t>28/02/2026</t>
   </si>
 </sst>
 </file>
@@ -536,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC914BC-115C-4E99-A655-A098063134BC}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -783,6 +792,58 @@
       </c>
       <c r="H14" s="4" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>